<commit_message>
corrected 2023 start date
</commit_message>
<xml_diff>
--- a/data/raw/hunting_seasons.xlsx
+++ b/data/raw/hunting_seasons.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\billy.DESKTOP-6FIO124\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\billy.DESKTOP-6FIO124\Documents\Master Thesis\raven_movement\data\raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0019C5B-14BA-4F87-A9AF-CC5E9BFA3A4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3619EB36-311F-40EB-8B65-E4F086DC4B9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{F8409187-CC4D-4331-8FBB-89995D232744}"/>
   </bookViews>
@@ -55,7 +55,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd;@"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -88,7 +88,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -426,7 +426,7 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -509,7 +509,7 @@
         <v>2023</v>
       </c>
       <c r="B6" s="1">
-        <v>45222</v>
+        <v>45220</v>
       </c>
       <c r="C6" s="1">
         <v>45256</v>

</xml_diff>

<commit_message>
fixing years for 2019
</commit_message>
<xml_diff>
--- a/data/raw/hunting_seasons.xlsx
+++ b/data/raw/hunting_seasons.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\billy.DESKTOP-6FIO124\Documents\Master Thesis\raven_movement\data\raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3619EB36-311F-40EB-8B65-E4F086DC4B9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{402FFD4F-40A1-46E7-86FC-97C968E28C7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{F8409187-CC4D-4331-8FBB-89995D232744}"/>
+    <workbookView xWindow="-25110" yWindow="3690" windowWidth="21600" windowHeight="11715" xr2:uid="{F8409187-CC4D-4331-8FBB-89995D232744}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -426,7 +426,7 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -453,13 +453,13 @@
         <v>2019</v>
       </c>
       <c r="B2" s="1">
-        <v>45591</v>
+        <v>43764</v>
       </c>
       <c r="C2" s="1">
-        <v>45627</v>
+        <v>43800</v>
       </c>
       <c r="D2" s="1">
-        <v>45613</v>
+        <v>43786</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">

</xml_diff>